<commit_message>
added cell type checks
</commit_message>
<xml_diff>
--- a/tests/data/validate_tables/no_description.xlsx
+++ b/tests/data/validate_tables/no_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedpreist/CodingStuff/DIMPACT/eam-data-tools/tests/data/validate_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A350E1-E1F9-8948-9203-0984DA27FBFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF5B4BA-16BA-9D40-8ED9-FA0BB55040A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="4540" windowWidth="23400" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>variable</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
+  </si>
+  <si>
+    <t>linear</t>
   </si>
 </sst>
 </file>
@@ -458,11 +464,13 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
     <col min="7" max="7" width="31.5" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
@@ -522,6 +530,12 @@
       </c>
       <c r="B3" t="s">
         <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>